<commit_message>
Removed special order cart function
</commit_message>
<xml_diff>
--- a/Project_Analysis_Team_3/Project_Analysis.xlsx
+++ b/Project_Analysis_Team_3/Project_Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houda/Desktop/UTA_Parking_reservation/Project_Analysis_Team_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houda/Desktop/UTA_Parking/Project_Analysis_Team_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E70C8FF-B0ED-144E-AA05-4158BD2179DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21441B14-FEAC-844A-99C5-6D3B13CA7EFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>Function ID</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Parking User</t>
-  </si>
-  <si>
-    <t>Special order cart</t>
-  </si>
-  <si>
-    <t>Parking user special orders cart outside of normal cart operation hours</t>
   </si>
   <si>
     <t>Admin</t>
@@ -415,11 +409,6 @@
   </si>
   <si>
     <t>Parking manager can modify a selected reservation.</t>
-  </si>
-  <si>
-    <t>Parking area name
-Pick up time
-Drop off time</t>
   </si>
   <si>
     <t>Username
@@ -497,7 +486,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,12 +502,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -586,16 +569,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -937,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG40"/>
+  <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -952,7 +925,7 @@
     <col min="5" max="5" width="31.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="40.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="1"/>
-    <col min="8" max="59" width="8.83203125" style="17"/>
+    <col min="8" max="59" width="8.83203125" style="13"/>
     <col min="60" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -975,77 +948,77 @@
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17"/>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-      <c r="BB1" s="17"/>
-      <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BB1" s="13"/>
+      <c r="BC1" s="13"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="13"/>
     </row>
     <row r="2" spans="1:59" ht="140">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:59" ht="60">
@@ -1065,7 +1038,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:59" ht="60">
@@ -1085,7 +1058,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:59" ht="140">
@@ -1096,16 +1069,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="160">
@@ -1113,19 +1086,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:59" ht="160">
@@ -1133,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>12</v>
@@ -1142,10 +1115,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:59" ht="100">
@@ -1153,7 +1126,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>12</v>
@@ -1162,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="40">
@@ -1173,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>12</v>
@@ -1185,7 +1158,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:59" ht="80">
@@ -1193,7 +1166,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>12</v>
@@ -1202,328 +1175,263 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" s="16" customFormat="1" ht="60">
-      <c r="A11" s="13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" ht="40">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="17"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="17"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="17"/>
-      <c r="AM11" s="17"/>
-      <c r="AN11" s="17"/>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="17"/>
-      <c r="AR11" s="17"/>
-      <c r="AS11" s="17"/>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="17"/>
-      <c r="AW11" s="17"/>
-      <c r="AX11" s="17"/>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="17"/>
-      <c r="BA11" s="17"/>
-      <c r="BB11" s="17"/>
-      <c r="BC11" s="17"/>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="17"/>
-      <c r="BF11" s="17"/>
-      <c r="BG11" s="17"/>
-    </row>
-    <row r="12" spans="1:59" ht="40">
+      <c r="B11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:59" ht="120">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:59" ht="120">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" ht="140">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:59" ht="140">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" ht="100">
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:59" ht="100">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" ht="120">
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:59" ht="120">
+    </row>
+    <row r="16" spans="1:59" ht="80">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="80">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="180">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="180">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="60">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="60">
+    <row r="19" spans="1:7" ht="140">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="140">
+    <row r="20" spans="1:7" ht="40">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="40">
+    </row>
+    <row r="21" spans="1:7" ht="120">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="120">
+        <v>71</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="140">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="140">
-      <c r="A23" s="8">
-        <v>22</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>77</v>
-      </c>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="B24" s="5"/>
@@ -1574,13 +1482,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1"/>
     <row r="32" spans="1:7" ht="15" customHeight="1"/>
     <row r="33" ht="15" customHeight="1"/>
     <row r="34" ht="15" customHeight="1"/>
@@ -1589,7 +1491,6 @@
     <row r="37" ht="15" customHeight="1"/>
     <row r="38" ht="15" customHeight="1"/>
     <row r="39" ht="15" customHeight="1"/>
-    <row r="40" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
My first push to GitHub :)
</commit_message>
<xml_diff>
--- a/Project_Analysis_Team_3/Project_Analysis.xlsx
+++ b/Project_Analysis_Team_3/Project_Analysis.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houda/Desktop/UTA_Parking/Project_Analysis_Team_3/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21441B14-FEAC-844A-99C5-6D3B13CA7EFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>Function ID</t>
   </si>
@@ -445,11 +439,14 @@
   <si>
     <t>Parking manager makes a particular spot unavailable/available starting from a particular time.</t>
   </si>
+  <si>
+    <t>Push to Gt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -632,7 +629,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,26 +662,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,23 +697,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -909,27 +872,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="22" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1"/>
-    <col min="8" max="59" width="8.83203125" style="13"/>
-    <col min="60" max="16384" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="31.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="59" width="8.85546875" style="13"/>
+    <col min="60" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="3" customFormat="1" ht="56" customHeight="1">
+    <row r="1" spans="1:59" s="3" customFormat="1" ht="56.1" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +964,7 @@
       <c r="BF1" s="13"/>
       <c r="BG1" s="13"/>
     </row>
-    <row r="2" spans="1:59" ht="140">
+    <row r="2" spans="1:59" ht="150">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1020,8 +983,11 @@
       <c r="F2" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:59" ht="60">
+      <c r="I2" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" ht="56.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1041,7 +1007,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="60">
+    <row r="4" spans="1:59" ht="56.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1061,7 +1027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="140">
+    <row r="5" spans="1:59" ht="131.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1081,7 +1047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="160">
+    <row r="6" spans="1:59" ht="168.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1101,7 +1067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="160">
+    <row r="7" spans="1:59" ht="150">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1121,7 +1087,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="100">
+    <row r="8" spans="1:59" ht="93.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1141,7 +1107,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="40">
+    <row r="9" spans="1:59" ht="37.5">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1161,7 +1127,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="80">
+    <row r="10" spans="1:59" ht="75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1181,7 +1147,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="40">
+    <row r="11" spans="1:59" ht="56.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1202,7 +1168,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:59" ht="120">
+    <row r="12" spans="1:59" ht="128.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1222,7 +1188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="140">
+    <row r="13" spans="1:59" ht="131.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1242,7 +1208,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="100">
+    <row r="14" spans="1:59" ht="112.5">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1262,7 +1228,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="120">
+    <row r="15" spans="1:59" ht="131.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1282,7 +1248,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="80">
+    <row r="16" spans="1:59" ht="75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1302,7 +1268,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="180">
+    <row r="17" spans="1:7" ht="167.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1323,7 +1289,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="60">
+    <row r="18" spans="1:7" ht="56.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1344,7 +1310,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="140">
+    <row r="19" spans="1:7" ht="131.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1365,7 +1331,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="40">
+    <row r="20" spans="1:7" ht="37.5">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1385,7 +1351,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="120">
+    <row r="21" spans="1:7" ht="112.5">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1406,7 +1372,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="140">
+    <row r="22" spans="1:7" ht="131.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1498,24 +1464,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reviewed validations and rules ppt
</commit_message>
<xml_diff>
--- a/Project_Analysis_Team_3/Project_Analysis.xlsx
+++ b/Project_Analysis_Team_3/Project_Analysis.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houda/Desktop/UTA_Parking/Project_Analysis_Team_3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA528D23-54E5-A646-8D9F-497C013E2948}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>Function ID</t>
   </si>
@@ -85,10 +91,6 @@
 Parking User</t>
   </si>
   <si>
-    <t>Time
-Type</t>
-  </si>
-  <si>
     <t>Register</t>
   </si>
   <si>
@@ -99,9 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">The non-admin user's profile information are displayed and can be modified. </t>
-  </si>
-  <si>
-    <t>System users fill in the registration form to sign up and selects the role as either Parking Manager, Parking User or Admin.</t>
   </si>
   <si>
     <t>Request reservation</t>
@@ -138,9 +137,6 @@
 Duration</t>
   </si>
   <si>
-    <t>Parking manager can search by UTA ID and view details of a specific parking user.</t>
-  </si>
-  <si>
     <t>View parking spot details</t>
   </si>
   <si>
@@ -197,19 +193,6 @@
 Options </t>
   </si>
   <si>
-    <t>Parking area name
-Spot number</t>
-  </si>
-  <si>
-    <t>A list of:
-Floor
-Parking type
-Occupancy status
-License plate
-Start time
-Duration</t>
-  </si>
-  <si>
     <t>Parking manager can view the details of a specific parking spot starting from current time as a list sorted in ascending order of start time</t>
   </si>
   <si>
@@ -217,9 +200,6 @@
   </si>
   <si>
     <t>Set violations</t>
-  </si>
-  <si>
-    <t>Parking manager sets no-show or overdue for parking user for that particular date</t>
   </si>
   <si>
     <t xml:space="preserve">Parking area name
@@ -274,29 +254,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>Number of floors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Total number of spots
-Parking types supported
-Options</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Username
 Role
 UTA ID
@@ -380,19 +337,7 @@
 One time fees (if incurred)</t>
   </si>
   <si>
-    <t>User name
-Password
-Role
-UTA ID
-Phone
-Email
-License plate number</t>
-  </si>
-  <si>
     <t>Parking manager makes a particular spot unavailable/available starting from a particular time.</t>
-  </si>
-  <si>
-    <t>Push to Gt</t>
   </si>
   <si>
     <t>Password
@@ -402,6 +347,12 @@
   </si>
   <si>
     <t>View my reservation status and violations</t>
+  </si>
+  <si>
+    <t>System users fills in the registration form to sign up and selects the role as either Parking Manager, Parking User or Admin.</t>
+  </si>
+  <si>
+    <t>Parking manager can search by username and view details of a specific parking user.</t>
   </si>
   <si>
     <r>
@@ -429,14 +380,68 @@
 Phone
 Email
 License number
-Status- active or revoked (reason for revocation)</t>
+Status- active or revoked 
+Reason for revocation</t>
     </r>
+  </si>
+  <si>
+    <t>Username
+Password
+Role
+UTA ID
+Phone
+Email
+License plate number</t>
+  </si>
+  <si>
+    <t>Time
+Parking type</t>
+  </si>
+  <si>
+    <t>A list of:
+Parking type
+Occupancy status
+License plate
+Start time
+Duration</t>
+  </si>
+  <si>
+    <t>Parking area name
+Spot number
+Floor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Parking name area
+Number of floors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Capacity
+Parking types supported
+Options</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Parking manager sets no-show or overdue for parking user. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -493,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -516,11 +521,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -550,14 +581,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,7 +671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,9 +704,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -687,6 +756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -862,25 +948,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG781"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="22" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="59" width="8.85546875" style="13"/>
-    <col min="60" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="31.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="48" style="18" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="59" width="8.83203125" style="12"/>
+    <col min="60" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="3" customFormat="1" ht="56.1" customHeight="1">
+    <row r="1" spans="1:59" s="3" customFormat="1" ht="56" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -893,89 +981,86 @@
       <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-    </row>
-    <row r="2" spans="1:59" ht="150">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+    </row>
+    <row r="2" spans="1:59" ht="161" customHeight="1">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:59" ht="56.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" ht="60">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -988,14 +1073,14 @@
       <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59" ht="56.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" ht="60">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1008,14 +1093,14 @@
       <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59" ht="75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" ht="80">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1028,39 +1113,39 @@
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>75</v>
+      <c r="E5" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" ht="168.75">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="160">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>71</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" ht="150">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" ht="160">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>12</v>
@@ -1068,14 +1153,14 @@
       <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>33</v>
+      <c r="E7" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59" ht="75">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" ht="80">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1088,14 +1173,14 @@
       <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>32</v>
+      <c r="E8" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59" ht="37.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" ht="40">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1108,19 +1193,19 @@
       <c r="D9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" ht="73.5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" ht="80">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>12</v>
@@ -1128,182 +1213,182 @@
       <c r="D10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" ht="56.25">
+    </row>
+    <row r="11" spans="1:59" ht="40">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:59" ht="128.25">
+    <row r="12" spans="1:59" ht="100">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>31</v>
+        <v>72</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:59" ht="131.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" ht="120">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:59" ht="112.5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" ht="100">
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>37</v>
+      <c r="B14" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:59" ht="131.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" ht="120">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:59" ht="75">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:59" ht="100">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>59</v>
+      <c r="D16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="167.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="180">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="56.25">
+    <row r="18" spans="1:7" ht="40">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="131.25">
+    <row r="19" spans="1:7" ht="140">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>14</v>
@@ -1311,15 +1396,15 @@
       <c r="D19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>49</v>
+      <c r="E19" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="37.5">
+    <row r="20" spans="1:7" ht="40">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1332,14 +1417,14 @@
       <c r="D20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="112.5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="120">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1352,15 +1437,15 @@
       <c r="D21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="150">
+    <row r="22" spans="1:7" ht="160">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1371,13 +1456,13 @@
         <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>77</v>
+        <v>62</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1">
@@ -1385,91 +1470,2338 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1"/>
-    <row r="32" spans="1:7" ht="15" customHeight="1"/>
-    <row r="33" ht="15" customHeight="1"/>
-    <row r="34" ht="15" customHeight="1"/>
-    <row r="35" ht="15" customHeight="1"/>
-    <row r="36" ht="15" customHeight="1"/>
-    <row r="37" ht="15" customHeight="1"/>
-    <row r="38" ht="15" customHeight="1"/>
-    <row r="39" ht="15" customHeight="1"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1">
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1">
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="6:6" ht="15" customHeight="1">
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="6:6" ht="15" customHeight="1">
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="6:6" ht="15" customHeight="1">
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="6:6" ht="15" customHeight="1">
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="6:6" ht="15" customHeight="1">
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="6:6" ht="15" customHeight="1">
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="6:6" ht="15" customHeight="1">
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="6:6">
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="6:6">
+      <c r="F41" s="20"/>
+    </row>
+    <row r="42" spans="6:6">
+      <c r="F42" s="20"/>
+    </row>
+    <row r="43" spans="6:6">
+      <c r="F43" s="20"/>
+    </row>
+    <row r="44" spans="6:6">
+      <c r="F44" s="20"/>
+    </row>
+    <row r="45" spans="6:6">
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="6:6">
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="6:6">
+      <c r="F47" s="20"/>
+    </row>
+    <row r="48" spans="6:6">
+      <c r="F48" s="20"/>
+    </row>
+    <row r="49" spans="6:6">
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="6:6">
+      <c r="F50" s="20"/>
+    </row>
+    <row r="51" spans="6:6">
+      <c r="F51" s="20"/>
+    </row>
+    <row r="52" spans="6:6">
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="6:6">
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="6:6">
+      <c r="F54" s="20"/>
+    </row>
+    <row r="55" spans="6:6">
+      <c r="F55" s="20"/>
+    </row>
+    <row r="56" spans="6:6">
+      <c r="F56" s="20"/>
+    </row>
+    <row r="57" spans="6:6">
+      <c r="F57" s="20"/>
+    </row>
+    <row r="58" spans="6:6">
+      <c r="F58" s="20"/>
+    </row>
+    <row r="59" spans="6:6">
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="6:6">
+      <c r="F60" s="20"/>
+    </row>
+    <row r="61" spans="6:6">
+      <c r="F61" s="20"/>
+    </row>
+    <row r="62" spans="6:6">
+      <c r="F62" s="20"/>
+    </row>
+    <row r="63" spans="6:6">
+      <c r="F63" s="20"/>
+    </row>
+    <row r="64" spans="6:6">
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="6:6">
+      <c r="F65" s="20"/>
+    </row>
+    <row r="66" spans="6:6">
+      <c r="F66" s="20"/>
+    </row>
+    <row r="67" spans="6:6">
+      <c r="F67" s="20"/>
+    </row>
+    <row r="68" spans="6:6">
+      <c r="F68" s="20"/>
+    </row>
+    <row r="69" spans="6:6">
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="6:6">
+      <c r="F70" s="20"/>
+    </row>
+    <row r="71" spans="6:6">
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="6:6">
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="6:6">
+      <c r="F73" s="20"/>
+    </row>
+    <row r="74" spans="6:6">
+      <c r="F74" s="20"/>
+    </row>
+    <row r="75" spans="6:6">
+      <c r="F75" s="20"/>
+    </row>
+    <row r="76" spans="6:6">
+      <c r="F76" s="20"/>
+    </row>
+    <row r="77" spans="6:6">
+      <c r="F77" s="20"/>
+    </row>
+    <row r="78" spans="6:6">
+      <c r="F78" s="20"/>
+    </row>
+    <row r="79" spans="6:6">
+      <c r="F79" s="20"/>
+    </row>
+    <row r="80" spans="6:6">
+      <c r="F80" s="20"/>
+    </row>
+    <row r="81" spans="6:6">
+      <c r="F81" s="20"/>
+    </row>
+    <row r="82" spans="6:6">
+      <c r="F82" s="20"/>
+    </row>
+    <row r="83" spans="6:6">
+      <c r="F83" s="20"/>
+    </row>
+    <row r="84" spans="6:6">
+      <c r="F84" s="20"/>
+    </row>
+    <row r="85" spans="6:6">
+      <c r="F85" s="20"/>
+    </row>
+    <row r="86" spans="6:6">
+      <c r="F86" s="20"/>
+    </row>
+    <row r="87" spans="6:6">
+      <c r="F87" s="20"/>
+    </row>
+    <row r="88" spans="6:6">
+      <c r="F88" s="20"/>
+    </row>
+    <row r="89" spans="6:6">
+      <c r="F89" s="20"/>
+    </row>
+    <row r="90" spans="6:6">
+      <c r="F90" s="20"/>
+    </row>
+    <row r="91" spans="6:6">
+      <c r="F91" s="20"/>
+    </row>
+    <row r="92" spans="6:6">
+      <c r="F92" s="20"/>
+    </row>
+    <row r="93" spans="6:6">
+      <c r="F93" s="20"/>
+    </row>
+    <row r="94" spans="6:6">
+      <c r="F94" s="20"/>
+    </row>
+    <row r="95" spans="6:6">
+      <c r="F95" s="20"/>
+    </row>
+    <row r="96" spans="6:6">
+      <c r="F96" s="20"/>
+    </row>
+    <row r="97" spans="6:6">
+      <c r="F97" s="20"/>
+    </row>
+    <row r="98" spans="6:6">
+      <c r="F98" s="20"/>
+    </row>
+    <row r="99" spans="6:6">
+      <c r="F99" s="20"/>
+    </row>
+    <row r="100" spans="6:6">
+      <c r="F100" s="20"/>
+    </row>
+    <row r="101" spans="6:6">
+      <c r="F101" s="20"/>
+    </row>
+    <row r="102" spans="6:6">
+      <c r="F102" s="20"/>
+    </row>
+    <row r="103" spans="6:6">
+      <c r="F103" s="20"/>
+    </row>
+    <row r="104" spans="6:6">
+      <c r="F104" s="20"/>
+    </row>
+    <row r="105" spans="6:6">
+      <c r="F105" s="20"/>
+    </row>
+    <row r="106" spans="6:6">
+      <c r="F106" s="20"/>
+    </row>
+    <row r="107" spans="6:6">
+      <c r="F107" s="20"/>
+    </row>
+    <row r="108" spans="6:6">
+      <c r="F108" s="20"/>
+    </row>
+    <row r="109" spans="6:6">
+      <c r="F109" s="20"/>
+    </row>
+    <row r="110" spans="6:6">
+      <c r="F110" s="20"/>
+    </row>
+    <row r="111" spans="6:6">
+      <c r="F111" s="20"/>
+    </row>
+    <row r="112" spans="6:6">
+      <c r="F112" s="20"/>
+    </row>
+    <row r="113" spans="6:6">
+      <c r="F113" s="20"/>
+    </row>
+    <row r="114" spans="6:6">
+      <c r="F114" s="20"/>
+    </row>
+    <row r="115" spans="6:6">
+      <c r="F115" s="20"/>
+    </row>
+    <row r="116" spans="6:6">
+      <c r="F116" s="20"/>
+    </row>
+    <row r="117" spans="6:6">
+      <c r="F117" s="20"/>
+    </row>
+    <row r="118" spans="6:6">
+      <c r="F118" s="20"/>
+    </row>
+    <row r="119" spans="6:6">
+      <c r="F119" s="20"/>
+    </row>
+    <row r="120" spans="6:6">
+      <c r="F120" s="20"/>
+    </row>
+    <row r="121" spans="6:6">
+      <c r="F121" s="20"/>
+    </row>
+    <row r="122" spans="6:6">
+      <c r="F122" s="20"/>
+    </row>
+    <row r="123" spans="6:6">
+      <c r="F123" s="20"/>
+    </row>
+    <row r="124" spans="6:6">
+      <c r="F124" s="20"/>
+    </row>
+    <row r="125" spans="6:6">
+      <c r="F125" s="20"/>
+    </row>
+    <row r="126" spans="6:6">
+      <c r="F126" s="20"/>
+    </row>
+    <row r="127" spans="6:6">
+      <c r="F127" s="20"/>
+    </row>
+    <row r="128" spans="6:6">
+      <c r="F128" s="20"/>
+    </row>
+    <row r="129" spans="6:6">
+      <c r="F129" s="20"/>
+    </row>
+    <row r="130" spans="6:6">
+      <c r="F130" s="20"/>
+    </row>
+    <row r="131" spans="6:6">
+      <c r="F131" s="20"/>
+    </row>
+    <row r="132" spans="6:6">
+      <c r="F132" s="20"/>
+    </row>
+    <row r="133" spans="6:6">
+      <c r="F133" s="20"/>
+    </row>
+    <row r="134" spans="6:6">
+      <c r="F134" s="20"/>
+    </row>
+    <row r="135" spans="6:6">
+      <c r="F135" s="20"/>
+    </row>
+    <row r="136" spans="6:6">
+      <c r="F136" s="20"/>
+    </row>
+    <row r="137" spans="6:6">
+      <c r="F137" s="20"/>
+    </row>
+    <row r="138" spans="6:6">
+      <c r="F138" s="20"/>
+    </row>
+    <row r="139" spans="6:6">
+      <c r="F139" s="20"/>
+    </row>
+    <row r="140" spans="6:6">
+      <c r="F140" s="20"/>
+    </row>
+    <row r="141" spans="6:6">
+      <c r="F141" s="20"/>
+    </row>
+    <row r="142" spans="6:6">
+      <c r="F142" s="20"/>
+    </row>
+    <row r="143" spans="6:6">
+      <c r="F143" s="20"/>
+    </row>
+    <row r="144" spans="6:6">
+      <c r="F144" s="20"/>
+    </row>
+    <row r="145" spans="6:6">
+      <c r="F145" s="20"/>
+    </row>
+    <row r="146" spans="6:6">
+      <c r="F146" s="20"/>
+    </row>
+    <row r="147" spans="6:6">
+      <c r="F147" s="20"/>
+    </row>
+    <row r="148" spans="6:6">
+      <c r="F148" s="20"/>
+    </row>
+    <row r="149" spans="6:6">
+      <c r="F149" s="20"/>
+    </row>
+    <row r="150" spans="6:6">
+      <c r="F150" s="20"/>
+    </row>
+    <row r="151" spans="6:6">
+      <c r="F151" s="20"/>
+    </row>
+    <row r="152" spans="6:6">
+      <c r="F152" s="20"/>
+    </row>
+    <row r="153" spans="6:6">
+      <c r="F153" s="20"/>
+    </row>
+    <row r="154" spans="6:6">
+      <c r="F154" s="20"/>
+    </row>
+    <row r="155" spans="6:6">
+      <c r="F155" s="20"/>
+    </row>
+    <row r="156" spans="6:6">
+      <c r="F156" s="20"/>
+    </row>
+    <row r="157" spans="6:6">
+      <c r="F157" s="20"/>
+    </row>
+    <row r="158" spans="6:6">
+      <c r="F158" s="20"/>
+    </row>
+    <row r="159" spans="6:6">
+      <c r="F159" s="20"/>
+    </row>
+    <row r="160" spans="6:6">
+      <c r="F160" s="20"/>
+    </row>
+    <row r="161" spans="6:6">
+      <c r="F161" s="20"/>
+    </row>
+    <row r="162" spans="6:6">
+      <c r="F162" s="20"/>
+    </row>
+    <row r="163" spans="6:6">
+      <c r="F163" s="20"/>
+    </row>
+    <row r="164" spans="6:6">
+      <c r="F164" s="20"/>
+    </row>
+    <row r="165" spans="6:6">
+      <c r="F165" s="20"/>
+    </row>
+    <row r="166" spans="6:6">
+      <c r="F166" s="20"/>
+    </row>
+    <row r="167" spans="6:6">
+      <c r="F167" s="20"/>
+    </row>
+    <row r="168" spans="6:6">
+      <c r="F168" s="20"/>
+    </row>
+    <row r="169" spans="6:6">
+      <c r="F169" s="20"/>
+    </row>
+    <row r="170" spans="6:6">
+      <c r="F170" s="20"/>
+    </row>
+    <row r="171" spans="6:6">
+      <c r="F171" s="20"/>
+    </row>
+    <row r="172" spans="6:6">
+      <c r="F172" s="20"/>
+    </row>
+    <row r="173" spans="6:6">
+      <c r="F173" s="20"/>
+    </row>
+    <row r="174" spans="6:6">
+      <c r="F174" s="20"/>
+    </row>
+    <row r="175" spans="6:6">
+      <c r="F175" s="20"/>
+    </row>
+    <row r="176" spans="6:6">
+      <c r="F176" s="20"/>
+    </row>
+    <row r="177" spans="6:6">
+      <c r="F177" s="20"/>
+    </row>
+    <row r="178" spans="6:6">
+      <c r="F178" s="20"/>
+    </row>
+    <row r="179" spans="6:6">
+      <c r="F179" s="20"/>
+    </row>
+    <row r="180" spans="6:6">
+      <c r="F180" s="20"/>
+    </row>
+    <row r="181" spans="6:6">
+      <c r="F181" s="20"/>
+    </row>
+    <row r="182" spans="6:6">
+      <c r="F182" s="20"/>
+    </row>
+    <row r="183" spans="6:6">
+      <c r="F183" s="20"/>
+    </row>
+    <row r="184" spans="6:6">
+      <c r="F184" s="20"/>
+    </row>
+    <row r="185" spans="6:6">
+      <c r="F185" s="20"/>
+    </row>
+    <row r="186" spans="6:6">
+      <c r="F186" s="20"/>
+    </row>
+    <row r="187" spans="6:6">
+      <c r="F187" s="20"/>
+    </row>
+    <row r="188" spans="6:6">
+      <c r="F188" s="20"/>
+    </row>
+    <row r="189" spans="6:6">
+      <c r="F189" s="20"/>
+    </row>
+    <row r="190" spans="6:6">
+      <c r="F190" s="20"/>
+    </row>
+    <row r="191" spans="6:6">
+      <c r="F191" s="20"/>
+    </row>
+    <row r="192" spans="6:6">
+      <c r="F192" s="20"/>
+    </row>
+    <row r="193" spans="6:6">
+      <c r="F193" s="20"/>
+    </row>
+    <row r="194" spans="6:6">
+      <c r="F194" s="20"/>
+    </row>
+    <row r="195" spans="6:6">
+      <c r="F195" s="20"/>
+    </row>
+    <row r="196" spans="6:6">
+      <c r="F196" s="20"/>
+    </row>
+    <row r="197" spans="6:6">
+      <c r="F197" s="20"/>
+    </row>
+    <row r="198" spans="6:6">
+      <c r="F198" s="20"/>
+    </row>
+    <row r="199" spans="6:6">
+      <c r="F199" s="20"/>
+    </row>
+    <row r="200" spans="6:6">
+      <c r="F200" s="20"/>
+    </row>
+    <row r="201" spans="6:6">
+      <c r="F201" s="20"/>
+    </row>
+    <row r="202" spans="6:6">
+      <c r="F202" s="20"/>
+    </row>
+    <row r="203" spans="6:6">
+      <c r="F203" s="20"/>
+    </row>
+    <row r="204" spans="6:6">
+      <c r="F204" s="20"/>
+    </row>
+    <row r="205" spans="6:6">
+      <c r="F205" s="20"/>
+    </row>
+    <row r="206" spans="6:6">
+      <c r="F206" s="20"/>
+    </row>
+    <row r="207" spans="6:6">
+      <c r="F207" s="20"/>
+    </row>
+    <row r="208" spans="6:6">
+      <c r="F208" s="20"/>
+    </row>
+    <row r="209" spans="6:6">
+      <c r="F209" s="20"/>
+    </row>
+    <row r="210" spans="6:6">
+      <c r="F210" s="20"/>
+    </row>
+    <row r="211" spans="6:6">
+      <c r="F211" s="20"/>
+    </row>
+    <row r="212" spans="6:6">
+      <c r="F212" s="20"/>
+    </row>
+    <row r="213" spans="6:6">
+      <c r="F213" s="20"/>
+    </row>
+    <row r="214" spans="6:6">
+      <c r="F214" s="20"/>
+    </row>
+    <row r="215" spans="6:6">
+      <c r="F215" s="20"/>
+    </row>
+    <row r="216" spans="6:6">
+      <c r="F216" s="20"/>
+    </row>
+    <row r="217" spans="6:6">
+      <c r="F217" s="20"/>
+    </row>
+    <row r="218" spans="6:6">
+      <c r="F218" s="20"/>
+    </row>
+    <row r="219" spans="6:6">
+      <c r="F219" s="20"/>
+    </row>
+    <row r="220" spans="6:6">
+      <c r="F220" s="20"/>
+    </row>
+    <row r="221" spans="6:6">
+      <c r="F221" s="20"/>
+    </row>
+    <row r="222" spans="6:6">
+      <c r="F222" s="20"/>
+    </row>
+    <row r="223" spans="6:6">
+      <c r="F223" s="20"/>
+    </row>
+    <row r="224" spans="6:6">
+      <c r="F224" s="20"/>
+    </row>
+    <row r="225" spans="6:6">
+      <c r="F225" s="20"/>
+    </row>
+    <row r="226" spans="6:6">
+      <c r="F226" s="20"/>
+    </row>
+    <row r="227" spans="6:6">
+      <c r="F227" s="20"/>
+    </row>
+    <row r="228" spans="6:6">
+      <c r="F228" s="20"/>
+    </row>
+    <row r="229" spans="6:6">
+      <c r="F229" s="20"/>
+    </row>
+    <row r="230" spans="6:6">
+      <c r="F230" s="20"/>
+    </row>
+    <row r="231" spans="6:6">
+      <c r="F231" s="20"/>
+    </row>
+    <row r="232" spans="6:6">
+      <c r="F232" s="20"/>
+    </row>
+    <row r="233" spans="6:6">
+      <c r="F233" s="20"/>
+    </row>
+    <row r="234" spans="6:6">
+      <c r="F234" s="20"/>
+    </row>
+    <row r="235" spans="6:6">
+      <c r="F235" s="20"/>
+    </row>
+    <row r="236" spans="6:6">
+      <c r="F236" s="20"/>
+    </row>
+    <row r="237" spans="6:6">
+      <c r="F237" s="20"/>
+    </row>
+    <row r="238" spans="6:6">
+      <c r="F238" s="20"/>
+    </row>
+    <row r="239" spans="6:6">
+      <c r="F239" s="20"/>
+    </row>
+    <row r="240" spans="6:6">
+      <c r="F240" s="20"/>
+    </row>
+    <row r="241" spans="6:6">
+      <c r="F241" s="20"/>
+    </row>
+    <row r="242" spans="6:6">
+      <c r="F242" s="20"/>
+    </row>
+    <row r="243" spans="6:6">
+      <c r="F243" s="20"/>
+    </row>
+    <row r="244" spans="6:6">
+      <c r="F244" s="20"/>
+    </row>
+    <row r="245" spans="6:6">
+      <c r="F245" s="20"/>
+    </row>
+    <row r="246" spans="6:6">
+      <c r="F246" s="20"/>
+    </row>
+    <row r="247" spans="6:6">
+      <c r="F247" s="20"/>
+    </row>
+    <row r="248" spans="6:6">
+      <c r="F248" s="20"/>
+    </row>
+    <row r="249" spans="6:6">
+      <c r="F249" s="20"/>
+    </row>
+    <row r="250" spans="6:6">
+      <c r="F250" s="20"/>
+    </row>
+    <row r="251" spans="6:6">
+      <c r="F251" s="20"/>
+    </row>
+    <row r="252" spans="6:6">
+      <c r="F252" s="20"/>
+    </row>
+    <row r="253" spans="6:6">
+      <c r="F253" s="20"/>
+    </row>
+    <row r="254" spans="6:6">
+      <c r="F254" s="20"/>
+    </row>
+    <row r="255" spans="6:6">
+      <c r="F255" s="20"/>
+    </row>
+    <row r="256" spans="6:6">
+      <c r="F256" s="20"/>
+    </row>
+    <row r="257" spans="6:6">
+      <c r="F257" s="20"/>
+    </row>
+    <row r="258" spans="6:6">
+      <c r="F258" s="20"/>
+    </row>
+    <row r="259" spans="6:6">
+      <c r="F259" s="20"/>
+    </row>
+    <row r="260" spans="6:6">
+      <c r="F260" s="20"/>
+    </row>
+    <row r="261" spans="6:6">
+      <c r="F261" s="20"/>
+    </row>
+    <row r="262" spans="6:6">
+      <c r="F262" s="20"/>
+    </row>
+    <row r="263" spans="6:6">
+      <c r="F263" s="20"/>
+    </row>
+    <row r="264" spans="6:6">
+      <c r="F264" s="20"/>
+    </row>
+    <row r="265" spans="6:6">
+      <c r="F265" s="20"/>
+    </row>
+    <row r="266" spans="6:6">
+      <c r="F266" s="20"/>
+    </row>
+    <row r="267" spans="6:6">
+      <c r="F267" s="20"/>
+    </row>
+    <row r="268" spans="6:6">
+      <c r="F268" s="20"/>
+    </row>
+    <row r="269" spans="6:6">
+      <c r="F269" s="20"/>
+    </row>
+    <row r="270" spans="6:6">
+      <c r="F270" s="20"/>
+    </row>
+    <row r="271" spans="6:6">
+      <c r="F271" s="20"/>
+    </row>
+    <row r="272" spans="6:6">
+      <c r="F272" s="20"/>
+    </row>
+    <row r="273" spans="6:6">
+      <c r="F273" s="20"/>
+    </row>
+    <row r="274" spans="6:6">
+      <c r="F274" s="20"/>
+    </row>
+    <row r="275" spans="6:6">
+      <c r="F275" s="20"/>
+    </row>
+    <row r="276" spans="6:6">
+      <c r="F276" s="20"/>
+    </row>
+    <row r="277" spans="6:6">
+      <c r="F277" s="20"/>
+    </row>
+    <row r="278" spans="6:6">
+      <c r="F278" s="20"/>
+    </row>
+    <row r="279" spans="6:6">
+      <c r="F279" s="20"/>
+    </row>
+    <row r="280" spans="6:6">
+      <c r="F280" s="20"/>
+    </row>
+    <row r="281" spans="6:6">
+      <c r="F281" s="20"/>
+    </row>
+    <row r="282" spans="6:6">
+      <c r="F282" s="20"/>
+    </row>
+    <row r="283" spans="6:6">
+      <c r="F283" s="20"/>
+    </row>
+    <row r="284" spans="6:6">
+      <c r="F284" s="20"/>
+    </row>
+    <row r="285" spans="6:6">
+      <c r="F285" s="20"/>
+    </row>
+    <row r="286" spans="6:6">
+      <c r="F286" s="20"/>
+    </row>
+    <row r="287" spans="6:6">
+      <c r="F287" s="20"/>
+    </row>
+    <row r="288" spans="6:6">
+      <c r="F288" s="20"/>
+    </row>
+    <row r="289" spans="6:6">
+      <c r="F289" s="20"/>
+    </row>
+    <row r="290" spans="6:6">
+      <c r="F290" s="20"/>
+    </row>
+    <row r="291" spans="6:6">
+      <c r="F291" s="20"/>
+    </row>
+    <row r="292" spans="6:6">
+      <c r="F292" s="20"/>
+    </row>
+    <row r="293" spans="6:6">
+      <c r="F293" s="20"/>
+    </row>
+    <row r="294" spans="6:6">
+      <c r="F294" s="20"/>
+    </row>
+    <row r="295" spans="6:6">
+      <c r="F295" s="20"/>
+    </row>
+    <row r="296" spans="6:6">
+      <c r="F296" s="20"/>
+    </row>
+    <row r="297" spans="6:6">
+      <c r="F297" s="20"/>
+    </row>
+    <row r="298" spans="6:6">
+      <c r="F298" s="20"/>
+    </row>
+    <row r="299" spans="6:6">
+      <c r="F299" s="20"/>
+    </row>
+    <row r="300" spans="6:6">
+      <c r="F300" s="20"/>
+    </row>
+    <row r="301" spans="6:6">
+      <c r="F301" s="20"/>
+    </row>
+    <row r="302" spans="6:6">
+      <c r="F302" s="20"/>
+    </row>
+    <row r="303" spans="6:6">
+      <c r="F303" s="20"/>
+    </row>
+    <row r="304" spans="6:6">
+      <c r="F304" s="20"/>
+    </row>
+    <row r="305" spans="6:6">
+      <c r="F305" s="20"/>
+    </row>
+    <row r="306" spans="6:6">
+      <c r="F306" s="20"/>
+    </row>
+    <row r="307" spans="6:6">
+      <c r="F307" s="20"/>
+    </row>
+    <row r="308" spans="6:6">
+      <c r="F308" s="20"/>
+    </row>
+    <row r="309" spans="6:6">
+      <c r="F309" s="20"/>
+    </row>
+    <row r="310" spans="6:6">
+      <c r="F310" s="20"/>
+    </row>
+    <row r="311" spans="6:6">
+      <c r="F311" s="20"/>
+    </row>
+    <row r="312" spans="6:6">
+      <c r="F312" s="20"/>
+    </row>
+    <row r="313" spans="6:6">
+      <c r="F313" s="20"/>
+    </row>
+    <row r="314" spans="6:6">
+      <c r="F314" s="20"/>
+    </row>
+    <row r="315" spans="6:6">
+      <c r="F315" s="20"/>
+    </row>
+    <row r="316" spans="6:6">
+      <c r="F316" s="20"/>
+    </row>
+    <row r="317" spans="6:6">
+      <c r="F317" s="20"/>
+    </row>
+    <row r="318" spans="6:6">
+      <c r="F318" s="20"/>
+    </row>
+    <row r="319" spans="6:6">
+      <c r="F319" s="20"/>
+    </row>
+    <row r="320" spans="6:6">
+      <c r="F320" s="20"/>
+    </row>
+    <row r="321" spans="6:6">
+      <c r="F321" s="20"/>
+    </row>
+    <row r="322" spans="6:6">
+      <c r="F322" s="20"/>
+    </row>
+    <row r="323" spans="6:6">
+      <c r="F323" s="20"/>
+    </row>
+    <row r="324" spans="6:6">
+      <c r="F324" s="20"/>
+    </row>
+    <row r="325" spans="6:6">
+      <c r="F325" s="20"/>
+    </row>
+    <row r="326" spans="6:6">
+      <c r="F326" s="20"/>
+    </row>
+    <row r="327" spans="6:6">
+      <c r="F327" s="20"/>
+    </row>
+    <row r="328" spans="6:6">
+      <c r="F328" s="20"/>
+    </row>
+    <row r="329" spans="6:6">
+      <c r="F329" s="20"/>
+    </row>
+    <row r="330" spans="6:6">
+      <c r="F330" s="20"/>
+    </row>
+    <row r="331" spans="6:6">
+      <c r="F331" s="20"/>
+    </row>
+    <row r="332" spans="6:6">
+      <c r="F332" s="20"/>
+    </row>
+    <row r="333" spans="6:6">
+      <c r="F333" s="20"/>
+    </row>
+    <row r="334" spans="6:6">
+      <c r="F334" s="20"/>
+    </row>
+    <row r="335" spans="6:6">
+      <c r="F335" s="20"/>
+    </row>
+    <row r="336" spans="6:6">
+      <c r="F336" s="20"/>
+    </row>
+    <row r="337" spans="6:6">
+      <c r="F337" s="20"/>
+    </row>
+    <row r="338" spans="6:6">
+      <c r="F338" s="20"/>
+    </row>
+    <row r="339" spans="6:6">
+      <c r="F339" s="20"/>
+    </row>
+    <row r="340" spans="6:6">
+      <c r="F340" s="20"/>
+    </row>
+    <row r="341" spans="6:6">
+      <c r="F341" s="20"/>
+    </row>
+    <row r="342" spans="6:6">
+      <c r="F342" s="20"/>
+    </row>
+    <row r="343" spans="6:6">
+      <c r="F343" s="20"/>
+    </row>
+    <row r="344" spans="6:6">
+      <c r="F344" s="20"/>
+    </row>
+    <row r="345" spans="6:6">
+      <c r="F345" s="20"/>
+    </row>
+    <row r="346" spans="6:6">
+      <c r="F346" s="20"/>
+    </row>
+    <row r="347" spans="6:6">
+      <c r="F347" s="20"/>
+    </row>
+    <row r="348" spans="6:6">
+      <c r="F348" s="20"/>
+    </row>
+    <row r="349" spans="6:6">
+      <c r="F349" s="20"/>
+    </row>
+    <row r="350" spans="6:6">
+      <c r="F350" s="20"/>
+    </row>
+    <row r="351" spans="6:6">
+      <c r="F351" s="20"/>
+    </row>
+    <row r="352" spans="6:6">
+      <c r="F352" s="20"/>
+    </row>
+    <row r="353" spans="6:6">
+      <c r="F353" s="20"/>
+    </row>
+    <row r="354" spans="6:6">
+      <c r="F354" s="20"/>
+    </row>
+    <row r="355" spans="6:6">
+      <c r="F355" s="20"/>
+    </row>
+    <row r="356" spans="6:6">
+      <c r="F356" s="20"/>
+    </row>
+    <row r="357" spans="6:6">
+      <c r="F357" s="20"/>
+    </row>
+    <row r="358" spans="6:6">
+      <c r="F358" s="20"/>
+    </row>
+    <row r="359" spans="6:6">
+      <c r="F359" s="20"/>
+    </row>
+    <row r="360" spans="6:6">
+      <c r="F360" s="20"/>
+    </row>
+    <row r="361" spans="6:6">
+      <c r="F361" s="20"/>
+    </row>
+    <row r="362" spans="6:6">
+      <c r="F362" s="20"/>
+    </row>
+    <row r="363" spans="6:6">
+      <c r="F363" s="20"/>
+    </row>
+    <row r="364" spans="6:6">
+      <c r="F364" s="20"/>
+    </row>
+    <row r="365" spans="6:6">
+      <c r="F365" s="20"/>
+    </row>
+    <row r="366" spans="6:6">
+      <c r="F366" s="20"/>
+    </row>
+    <row r="367" spans="6:6">
+      <c r="F367" s="20"/>
+    </row>
+    <row r="368" spans="6:6">
+      <c r="F368" s="20"/>
+    </row>
+    <row r="369" spans="6:6">
+      <c r="F369" s="20"/>
+    </row>
+    <row r="370" spans="6:6">
+      <c r="F370" s="20"/>
+    </row>
+    <row r="371" spans="6:6">
+      <c r="F371" s="20"/>
+    </row>
+    <row r="372" spans="6:6">
+      <c r="F372" s="20"/>
+    </row>
+    <row r="373" spans="6:6">
+      <c r="F373" s="20"/>
+    </row>
+    <row r="374" spans="6:6">
+      <c r="F374" s="20"/>
+    </row>
+    <row r="375" spans="6:6">
+      <c r="F375" s="20"/>
+    </row>
+    <row r="376" spans="6:6">
+      <c r="F376" s="20"/>
+    </row>
+    <row r="377" spans="6:6">
+      <c r="F377" s="20"/>
+    </row>
+    <row r="378" spans="6:6">
+      <c r="F378" s="20"/>
+    </row>
+    <row r="379" spans="6:6">
+      <c r="F379" s="20"/>
+    </row>
+    <row r="380" spans="6:6">
+      <c r="F380" s="20"/>
+    </row>
+    <row r="381" spans="6:6">
+      <c r="F381" s="20"/>
+    </row>
+    <row r="382" spans="6:6">
+      <c r="F382" s="20"/>
+    </row>
+    <row r="383" spans="6:6">
+      <c r="F383" s="20"/>
+    </row>
+    <row r="384" spans="6:6">
+      <c r="F384" s="20"/>
+    </row>
+    <row r="385" spans="6:6">
+      <c r="F385" s="20"/>
+    </row>
+    <row r="386" spans="6:6">
+      <c r="F386" s="20"/>
+    </row>
+    <row r="387" spans="6:6">
+      <c r="F387" s="20"/>
+    </row>
+    <row r="388" spans="6:6">
+      <c r="F388" s="20"/>
+    </row>
+    <row r="389" spans="6:6">
+      <c r="F389" s="20"/>
+    </row>
+    <row r="390" spans="6:6">
+      <c r="F390" s="20"/>
+    </row>
+    <row r="391" spans="6:6">
+      <c r="F391" s="20"/>
+    </row>
+    <row r="392" spans="6:6">
+      <c r="F392" s="20"/>
+    </row>
+    <row r="393" spans="6:6">
+      <c r="F393" s="20"/>
+    </row>
+    <row r="394" spans="6:6">
+      <c r="F394" s="20"/>
+    </row>
+    <row r="395" spans="6:6">
+      <c r="F395" s="20"/>
+    </row>
+    <row r="396" spans="6:6">
+      <c r="F396" s="20"/>
+    </row>
+    <row r="397" spans="6:6">
+      <c r="F397" s="20"/>
+    </row>
+    <row r="398" spans="6:6">
+      <c r="F398" s="20"/>
+    </row>
+    <row r="399" spans="6:6">
+      <c r="F399" s="20"/>
+    </row>
+    <row r="400" spans="6:6">
+      <c r="F400" s="20"/>
+    </row>
+    <row r="401" spans="6:6">
+      <c r="F401" s="20"/>
+    </row>
+    <row r="402" spans="6:6">
+      <c r="F402" s="20"/>
+    </row>
+    <row r="403" spans="6:6">
+      <c r="F403" s="20"/>
+    </row>
+    <row r="404" spans="6:6">
+      <c r="F404" s="20"/>
+    </row>
+    <row r="405" spans="6:6">
+      <c r="F405" s="20"/>
+    </row>
+    <row r="406" spans="6:6">
+      <c r="F406" s="20"/>
+    </row>
+    <row r="407" spans="6:6">
+      <c r="F407" s="20"/>
+    </row>
+    <row r="408" spans="6:6">
+      <c r="F408" s="20"/>
+    </row>
+    <row r="409" spans="6:6">
+      <c r="F409" s="20"/>
+    </row>
+    <row r="410" spans="6:6">
+      <c r="F410" s="20"/>
+    </row>
+    <row r="411" spans="6:6">
+      <c r="F411" s="20"/>
+    </row>
+    <row r="412" spans="6:6">
+      <c r="F412" s="20"/>
+    </row>
+    <row r="413" spans="6:6">
+      <c r="F413" s="20"/>
+    </row>
+    <row r="414" spans="6:6">
+      <c r="F414" s="20"/>
+    </row>
+    <row r="415" spans="6:6">
+      <c r="F415" s="20"/>
+    </row>
+    <row r="416" spans="6:6">
+      <c r="F416" s="20"/>
+    </row>
+    <row r="417" spans="6:6">
+      <c r="F417" s="20"/>
+    </row>
+    <row r="418" spans="6:6">
+      <c r="F418" s="20"/>
+    </row>
+    <row r="419" spans="6:6">
+      <c r="F419" s="20"/>
+    </row>
+    <row r="420" spans="6:6">
+      <c r="F420" s="20"/>
+    </row>
+    <row r="421" spans="6:6">
+      <c r="F421" s="20"/>
+    </row>
+    <row r="422" spans="6:6">
+      <c r="F422" s="20"/>
+    </row>
+    <row r="423" spans="6:6">
+      <c r="F423" s="20"/>
+    </row>
+    <row r="424" spans="6:6">
+      <c r="F424" s="20"/>
+    </row>
+    <row r="425" spans="6:6">
+      <c r="F425" s="20"/>
+    </row>
+    <row r="426" spans="6:6">
+      <c r="F426" s="20"/>
+    </row>
+    <row r="427" spans="6:6">
+      <c r="F427" s="20"/>
+    </row>
+    <row r="428" spans="6:6">
+      <c r="F428" s="20"/>
+    </row>
+    <row r="429" spans="6:6">
+      <c r="F429" s="20"/>
+    </row>
+    <row r="430" spans="6:6">
+      <c r="F430" s="20"/>
+    </row>
+    <row r="431" spans="6:6">
+      <c r="F431" s="20"/>
+    </row>
+    <row r="432" spans="6:6">
+      <c r="F432" s="20"/>
+    </row>
+    <row r="433" spans="6:6">
+      <c r="F433" s="20"/>
+    </row>
+    <row r="434" spans="6:6">
+      <c r="F434" s="20"/>
+    </row>
+    <row r="435" spans="6:6">
+      <c r="F435" s="20"/>
+    </row>
+    <row r="436" spans="6:6">
+      <c r="F436" s="20"/>
+    </row>
+    <row r="437" spans="6:6">
+      <c r="F437" s="20"/>
+    </row>
+    <row r="438" spans="6:6">
+      <c r="F438" s="20"/>
+    </row>
+    <row r="439" spans="6:6">
+      <c r="F439" s="20"/>
+    </row>
+    <row r="440" spans="6:6">
+      <c r="F440" s="20"/>
+    </row>
+    <row r="441" spans="6:6">
+      <c r="F441" s="20"/>
+    </row>
+    <row r="442" spans="6:6">
+      <c r="F442" s="20"/>
+    </row>
+    <row r="443" spans="6:6">
+      <c r="F443" s="20"/>
+    </row>
+    <row r="444" spans="6:6">
+      <c r="F444" s="20"/>
+    </row>
+    <row r="445" spans="6:6">
+      <c r="F445" s="20"/>
+    </row>
+    <row r="446" spans="6:6">
+      <c r="F446" s="20"/>
+    </row>
+    <row r="447" spans="6:6">
+      <c r="F447" s="20"/>
+    </row>
+    <row r="448" spans="6:6">
+      <c r="F448" s="20"/>
+    </row>
+    <row r="449" spans="6:6">
+      <c r="F449" s="20"/>
+    </row>
+    <row r="450" spans="6:6">
+      <c r="F450" s="20"/>
+    </row>
+    <row r="451" spans="6:6">
+      <c r="F451" s="20"/>
+    </row>
+    <row r="452" spans="6:6">
+      <c r="F452" s="20"/>
+    </row>
+    <row r="453" spans="6:6">
+      <c r="F453" s="20"/>
+    </row>
+    <row r="454" spans="6:6">
+      <c r="F454" s="20"/>
+    </row>
+    <row r="455" spans="6:6">
+      <c r="F455" s="20"/>
+    </row>
+    <row r="456" spans="6:6">
+      <c r="F456" s="20"/>
+    </row>
+    <row r="457" spans="6:6">
+      <c r="F457" s="20"/>
+    </row>
+    <row r="458" spans="6:6">
+      <c r="F458" s="20"/>
+    </row>
+    <row r="459" spans="6:6">
+      <c r="F459" s="20"/>
+    </row>
+    <row r="460" spans="6:6">
+      <c r="F460" s="20"/>
+    </row>
+    <row r="461" spans="6:6">
+      <c r="F461" s="20"/>
+    </row>
+    <row r="462" spans="6:6">
+      <c r="F462" s="20"/>
+    </row>
+    <row r="463" spans="6:6">
+      <c r="F463" s="20"/>
+    </row>
+    <row r="464" spans="6:6">
+      <c r="F464" s="20"/>
+    </row>
+    <row r="465" spans="6:6">
+      <c r="F465" s="20"/>
+    </row>
+    <row r="466" spans="6:6">
+      <c r="F466" s="20"/>
+    </row>
+    <row r="467" spans="6:6">
+      <c r="F467" s="20"/>
+    </row>
+    <row r="468" spans="6:6">
+      <c r="F468" s="20"/>
+    </row>
+    <row r="469" spans="6:6">
+      <c r="F469" s="20"/>
+    </row>
+    <row r="470" spans="6:6">
+      <c r="F470" s="20"/>
+    </row>
+    <row r="471" spans="6:6">
+      <c r="F471" s="20"/>
+    </row>
+    <row r="472" spans="6:6">
+      <c r="F472" s="20"/>
+    </row>
+    <row r="473" spans="6:6">
+      <c r="F473" s="20"/>
+    </row>
+    <row r="474" spans="6:6">
+      <c r="F474" s="20"/>
+    </row>
+    <row r="475" spans="6:6">
+      <c r="F475" s="20"/>
+    </row>
+    <row r="476" spans="6:6">
+      <c r="F476" s="20"/>
+    </row>
+    <row r="477" spans="6:6">
+      <c r="F477" s="20"/>
+    </row>
+    <row r="478" spans="6:6">
+      <c r="F478" s="20"/>
+    </row>
+    <row r="479" spans="6:6">
+      <c r="F479" s="20"/>
+    </row>
+    <row r="480" spans="6:6">
+      <c r="F480" s="20"/>
+    </row>
+    <row r="481" spans="6:6">
+      <c r="F481" s="20"/>
+    </row>
+    <row r="482" spans="6:6">
+      <c r="F482" s="20"/>
+    </row>
+    <row r="483" spans="6:6">
+      <c r="F483" s="20"/>
+    </row>
+    <row r="484" spans="6:6">
+      <c r="F484" s="20"/>
+    </row>
+    <row r="485" spans="6:6">
+      <c r="F485" s="20"/>
+    </row>
+    <row r="486" spans="6:6">
+      <c r="F486" s="20"/>
+    </row>
+    <row r="487" spans="6:6">
+      <c r="F487" s="20"/>
+    </row>
+    <row r="488" spans="6:6">
+      <c r="F488" s="20"/>
+    </row>
+    <row r="489" spans="6:6">
+      <c r="F489" s="20"/>
+    </row>
+    <row r="490" spans="6:6">
+      <c r="F490" s="20"/>
+    </row>
+    <row r="491" spans="6:6">
+      <c r="F491" s="20"/>
+    </row>
+    <row r="492" spans="6:6">
+      <c r="F492" s="20"/>
+    </row>
+    <row r="493" spans="6:6">
+      <c r="F493" s="20"/>
+    </row>
+    <row r="494" spans="6:6">
+      <c r="F494" s="20"/>
+    </row>
+    <row r="495" spans="6:6">
+      <c r="F495" s="20"/>
+    </row>
+    <row r="496" spans="6:6">
+      <c r="F496" s="20"/>
+    </row>
+    <row r="497" spans="6:6">
+      <c r="F497" s="20"/>
+    </row>
+    <row r="498" spans="6:6">
+      <c r="F498" s="20"/>
+    </row>
+    <row r="499" spans="6:6">
+      <c r="F499" s="20"/>
+    </row>
+    <row r="500" spans="6:6">
+      <c r="F500" s="20"/>
+    </row>
+    <row r="501" spans="6:6">
+      <c r="F501" s="20"/>
+    </row>
+    <row r="502" spans="6:6">
+      <c r="F502" s="20"/>
+    </row>
+    <row r="503" spans="6:6">
+      <c r="F503" s="20"/>
+    </row>
+    <row r="504" spans="6:6">
+      <c r="F504" s="20"/>
+    </row>
+    <row r="505" spans="6:6">
+      <c r="F505" s="20"/>
+    </row>
+    <row r="506" spans="6:6">
+      <c r="F506" s="20"/>
+    </row>
+    <row r="507" spans="6:6">
+      <c r="F507" s="20"/>
+    </row>
+    <row r="508" spans="6:6">
+      <c r="F508" s="20"/>
+    </row>
+    <row r="509" spans="6:6">
+      <c r="F509" s="20"/>
+    </row>
+    <row r="510" spans="6:6">
+      <c r="F510" s="20"/>
+    </row>
+    <row r="511" spans="6:6">
+      <c r="F511" s="20"/>
+    </row>
+    <row r="512" spans="6:6">
+      <c r="F512" s="20"/>
+    </row>
+    <row r="513" spans="6:6">
+      <c r="F513" s="20"/>
+    </row>
+    <row r="514" spans="6:6">
+      <c r="F514" s="20"/>
+    </row>
+    <row r="515" spans="6:6">
+      <c r="F515" s="20"/>
+    </row>
+    <row r="516" spans="6:6">
+      <c r="F516" s="20"/>
+    </row>
+    <row r="517" spans="6:6">
+      <c r="F517" s="20"/>
+    </row>
+    <row r="518" spans="6:6">
+      <c r="F518" s="20"/>
+    </row>
+    <row r="519" spans="6:6">
+      <c r="F519" s="20"/>
+    </row>
+    <row r="520" spans="6:6">
+      <c r="F520" s="20"/>
+    </row>
+    <row r="521" spans="6:6">
+      <c r="F521" s="20"/>
+    </row>
+    <row r="522" spans="6:6">
+      <c r="F522" s="20"/>
+    </row>
+    <row r="523" spans="6:6">
+      <c r="F523" s="20"/>
+    </row>
+    <row r="524" spans="6:6">
+      <c r="F524" s="20"/>
+    </row>
+    <row r="525" spans="6:6">
+      <c r="F525" s="20"/>
+    </row>
+    <row r="526" spans="6:6">
+      <c r="F526" s="20"/>
+    </row>
+    <row r="527" spans="6:6">
+      <c r="F527" s="20"/>
+    </row>
+    <row r="528" spans="6:6">
+      <c r="F528" s="20"/>
+    </row>
+    <row r="529" spans="6:6">
+      <c r="F529" s="20"/>
+    </row>
+    <row r="530" spans="6:6">
+      <c r="F530" s="20"/>
+    </row>
+    <row r="531" spans="6:6">
+      <c r="F531" s="20"/>
+    </row>
+    <row r="532" spans="6:6">
+      <c r="F532" s="20"/>
+    </row>
+    <row r="533" spans="6:6">
+      <c r="F533" s="20"/>
+    </row>
+    <row r="534" spans="6:6">
+      <c r="F534" s="20"/>
+    </row>
+    <row r="535" spans="6:6">
+      <c r="F535" s="20"/>
+    </row>
+    <row r="536" spans="6:6">
+      <c r="F536" s="20"/>
+    </row>
+    <row r="537" spans="6:6">
+      <c r="F537" s="20"/>
+    </row>
+    <row r="538" spans="6:6">
+      <c r="F538" s="20"/>
+    </row>
+    <row r="539" spans="6:6">
+      <c r="F539" s="20"/>
+    </row>
+    <row r="540" spans="6:6">
+      <c r="F540" s="20"/>
+    </row>
+    <row r="541" spans="6:6">
+      <c r="F541" s="20"/>
+    </row>
+    <row r="542" spans="6:6">
+      <c r="F542" s="20"/>
+    </row>
+    <row r="543" spans="6:6">
+      <c r="F543" s="20"/>
+    </row>
+    <row r="544" spans="6:6">
+      <c r="F544" s="20"/>
+    </row>
+    <row r="545" spans="6:6">
+      <c r="F545" s="20"/>
+    </row>
+    <row r="546" spans="6:6">
+      <c r="F546" s="20"/>
+    </row>
+    <row r="547" spans="6:6">
+      <c r="F547" s="20"/>
+    </row>
+    <row r="548" spans="6:6">
+      <c r="F548" s="20"/>
+    </row>
+    <row r="549" spans="6:6">
+      <c r="F549" s="20"/>
+    </row>
+    <row r="550" spans="6:6">
+      <c r="F550" s="20"/>
+    </row>
+    <row r="551" spans="6:6">
+      <c r="F551" s="20"/>
+    </row>
+    <row r="552" spans="6:6">
+      <c r="F552" s="20"/>
+    </row>
+    <row r="553" spans="6:6">
+      <c r="F553" s="20"/>
+    </row>
+    <row r="554" spans="6:6">
+      <c r="F554" s="20"/>
+    </row>
+    <row r="555" spans="6:6">
+      <c r="F555" s="20"/>
+    </row>
+    <row r="556" spans="6:6">
+      <c r="F556" s="20"/>
+    </row>
+    <row r="557" spans="6:6">
+      <c r="F557" s="20"/>
+    </row>
+    <row r="558" spans="6:6">
+      <c r="F558" s="20"/>
+    </row>
+    <row r="559" spans="6:6">
+      <c r="F559" s="20"/>
+    </row>
+    <row r="560" spans="6:6">
+      <c r="F560" s="20"/>
+    </row>
+    <row r="561" spans="6:6">
+      <c r="F561" s="20"/>
+    </row>
+    <row r="562" spans="6:6">
+      <c r="F562" s="20"/>
+    </row>
+    <row r="563" spans="6:6">
+      <c r="F563" s="20"/>
+    </row>
+    <row r="564" spans="6:6">
+      <c r="F564" s="20"/>
+    </row>
+    <row r="565" spans="6:6">
+      <c r="F565" s="20"/>
+    </row>
+    <row r="566" spans="6:6">
+      <c r="F566" s="20"/>
+    </row>
+    <row r="567" spans="6:6">
+      <c r="F567" s="20"/>
+    </row>
+    <row r="568" spans="6:6">
+      <c r="F568" s="20"/>
+    </row>
+    <row r="569" spans="6:6">
+      <c r="F569" s="20"/>
+    </row>
+    <row r="570" spans="6:6">
+      <c r="F570" s="20"/>
+    </row>
+    <row r="571" spans="6:6">
+      <c r="F571" s="20"/>
+    </row>
+    <row r="572" spans="6:6">
+      <c r="F572" s="20"/>
+    </row>
+    <row r="573" spans="6:6">
+      <c r="F573" s="20"/>
+    </row>
+    <row r="574" spans="6:6">
+      <c r="F574" s="20"/>
+    </row>
+    <row r="575" spans="6:6">
+      <c r="F575" s="20"/>
+    </row>
+    <row r="576" spans="6:6">
+      <c r="F576" s="20"/>
+    </row>
+    <row r="577" spans="6:6">
+      <c r="F577" s="20"/>
+    </row>
+    <row r="578" spans="6:6">
+      <c r="F578" s="20"/>
+    </row>
+    <row r="579" spans="6:6">
+      <c r="F579" s="20"/>
+    </row>
+    <row r="580" spans="6:6">
+      <c r="F580" s="20"/>
+    </row>
+    <row r="581" spans="6:6">
+      <c r="F581" s="20"/>
+    </row>
+    <row r="582" spans="6:6">
+      <c r="F582" s="20"/>
+    </row>
+    <row r="583" spans="6:6">
+      <c r="F583" s="20"/>
+    </row>
+    <row r="584" spans="6:6">
+      <c r="F584" s="20"/>
+    </row>
+    <row r="585" spans="6:6">
+      <c r="F585" s="20"/>
+    </row>
+    <row r="586" spans="6:6">
+      <c r="F586" s="20"/>
+    </row>
+    <row r="587" spans="6:6">
+      <c r="F587" s="20"/>
+    </row>
+    <row r="588" spans="6:6">
+      <c r="F588" s="20"/>
+    </row>
+    <row r="589" spans="6:6">
+      <c r="F589" s="20"/>
+    </row>
+    <row r="590" spans="6:6">
+      <c r="F590" s="20"/>
+    </row>
+    <row r="591" spans="6:6">
+      <c r="F591" s="20"/>
+    </row>
+    <row r="592" spans="6:6">
+      <c r="F592" s="20"/>
+    </row>
+    <row r="593" spans="6:6">
+      <c r="F593" s="20"/>
+    </row>
+    <row r="594" spans="6:6">
+      <c r="F594" s="20"/>
+    </row>
+    <row r="595" spans="6:6">
+      <c r="F595" s="20"/>
+    </row>
+    <row r="596" spans="6:6">
+      <c r="F596" s="20"/>
+    </row>
+    <row r="597" spans="6:6">
+      <c r="F597" s="20"/>
+    </row>
+    <row r="598" spans="6:6">
+      <c r="F598" s="20"/>
+    </row>
+    <row r="599" spans="6:6">
+      <c r="F599" s="20"/>
+    </row>
+    <row r="600" spans="6:6">
+      <c r="F600" s="20"/>
+    </row>
+    <row r="601" spans="6:6">
+      <c r="F601" s="20"/>
+    </row>
+    <row r="602" spans="6:6">
+      <c r="F602" s="20"/>
+    </row>
+    <row r="603" spans="6:6">
+      <c r="F603" s="20"/>
+    </row>
+    <row r="604" spans="6:6">
+      <c r="F604" s="20"/>
+    </row>
+    <row r="605" spans="6:6">
+      <c r="F605" s="20"/>
+    </row>
+    <row r="606" spans="6:6">
+      <c r="F606" s="20"/>
+    </row>
+    <row r="607" spans="6:6">
+      <c r="F607" s="20"/>
+    </row>
+    <row r="608" spans="6:6">
+      <c r="F608" s="20"/>
+    </row>
+    <row r="609" spans="6:6">
+      <c r="F609" s="20"/>
+    </row>
+    <row r="610" spans="6:6">
+      <c r="F610" s="20"/>
+    </row>
+    <row r="611" spans="6:6">
+      <c r="F611" s="20"/>
+    </row>
+    <row r="612" spans="6:6">
+      <c r="F612" s="20"/>
+    </row>
+    <row r="613" spans="6:6">
+      <c r="F613" s="20"/>
+    </row>
+    <row r="614" spans="6:6">
+      <c r="F614" s="20"/>
+    </row>
+    <row r="615" spans="6:6">
+      <c r="F615" s="20"/>
+    </row>
+    <row r="616" spans="6:6">
+      <c r="F616" s="20"/>
+    </row>
+    <row r="617" spans="6:6">
+      <c r="F617" s="20"/>
+    </row>
+    <row r="618" spans="6:6">
+      <c r="F618" s="20"/>
+    </row>
+    <row r="619" spans="6:6">
+      <c r="F619" s="20"/>
+    </row>
+    <row r="620" spans="6:6">
+      <c r="F620" s="20"/>
+    </row>
+    <row r="621" spans="6:6">
+      <c r="F621" s="20"/>
+    </row>
+    <row r="622" spans="6:6">
+      <c r="F622" s="20"/>
+    </row>
+    <row r="623" spans="6:6">
+      <c r="F623" s="20"/>
+    </row>
+    <row r="624" spans="6:6">
+      <c r="F624" s="20"/>
+    </row>
+    <row r="625" spans="6:6">
+      <c r="F625" s="20"/>
+    </row>
+    <row r="626" spans="6:6">
+      <c r="F626" s="20"/>
+    </row>
+    <row r="627" spans="6:6">
+      <c r="F627" s="20"/>
+    </row>
+    <row r="628" spans="6:6">
+      <c r="F628" s="20"/>
+    </row>
+    <row r="629" spans="6:6">
+      <c r="F629" s="20"/>
+    </row>
+    <row r="630" spans="6:6">
+      <c r="F630" s="20"/>
+    </row>
+    <row r="631" spans="6:6">
+      <c r="F631" s="20"/>
+    </row>
+    <row r="632" spans="6:6">
+      <c r="F632" s="20"/>
+    </row>
+    <row r="633" spans="6:6">
+      <c r="F633" s="20"/>
+    </row>
+    <row r="634" spans="6:6">
+      <c r="F634" s="20"/>
+    </row>
+    <row r="635" spans="6:6">
+      <c r="F635" s="20"/>
+    </row>
+    <row r="636" spans="6:6">
+      <c r="F636" s="20"/>
+    </row>
+    <row r="637" spans="6:6">
+      <c r="F637" s="20"/>
+    </row>
+    <row r="638" spans="6:6">
+      <c r="F638" s="20"/>
+    </row>
+    <row r="639" spans="6:6">
+      <c r="F639" s="20"/>
+    </row>
+    <row r="640" spans="6:6">
+      <c r="F640" s="20"/>
+    </row>
+    <row r="641" spans="6:6">
+      <c r="F641" s="20"/>
+    </row>
+    <row r="642" spans="6:6">
+      <c r="F642" s="20"/>
+    </row>
+    <row r="643" spans="6:6">
+      <c r="F643" s="20"/>
+    </row>
+    <row r="644" spans="6:6">
+      <c r="F644" s="20"/>
+    </row>
+    <row r="645" spans="6:6">
+      <c r="F645" s="20"/>
+    </row>
+    <row r="646" spans="6:6">
+      <c r="F646" s="20"/>
+    </row>
+    <row r="647" spans="6:6">
+      <c r="F647" s="20"/>
+    </row>
+    <row r="648" spans="6:6">
+      <c r="F648" s="20"/>
+    </row>
+    <row r="649" spans="6:6">
+      <c r="F649" s="20"/>
+    </row>
+    <row r="650" spans="6:6">
+      <c r="F650" s="20"/>
+    </row>
+    <row r="651" spans="6:6">
+      <c r="F651" s="20"/>
+    </row>
+    <row r="652" spans="6:6">
+      <c r="F652" s="20"/>
+    </row>
+    <row r="653" spans="6:6">
+      <c r="F653" s="20"/>
+    </row>
+    <row r="654" spans="6:6">
+      <c r="F654" s="20"/>
+    </row>
+    <row r="655" spans="6:6">
+      <c r="F655" s="20"/>
+    </row>
+    <row r="656" spans="6:6">
+      <c r="F656" s="20"/>
+    </row>
+    <row r="657" spans="6:6">
+      <c r="F657" s="20"/>
+    </row>
+    <row r="658" spans="6:6">
+      <c r="F658" s="20"/>
+    </row>
+    <row r="659" spans="6:6">
+      <c r="F659" s="20"/>
+    </row>
+    <row r="660" spans="6:6">
+      <c r="F660" s="20"/>
+    </row>
+    <row r="661" spans="6:6">
+      <c r="F661" s="20"/>
+    </row>
+    <row r="662" spans="6:6">
+      <c r="F662" s="20"/>
+    </row>
+    <row r="663" spans="6:6">
+      <c r="F663" s="20"/>
+    </row>
+    <row r="664" spans="6:6">
+      <c r="F664" s="20"/>
+    </row>
+    <row r="665" spans="6:6">
+      <c r="F665" s="20"/>
+    </row>
+    <row r="666" spans="6:6">
+      <c r="F666" s="20"/>
+    </row>
+    <row r="667" spans="6:6">
+      <c r="F667" s="20"/>
+    </row>
+    <row r="668" spans="6:6">
+      <c r="F668" s="20"/>
+    </row>
+    <row r="669" spans="6:6">
+      <c r="F669" s="20"/>
+    </row>
+    <row r="670" spans="6:6">
+      <c r="F670" s="20"/>
+    </row>
+    <row r="671" spans="6:6">
+      <c r="F671" s="20"/>
+    </row>
+    <row r="672" spans="6:6">
+      <c r="F672" s="20"/>
+    </row>
+    <row r="673" spans="6:6">
+      <c r="F673" s="20"/>
+    </row>
+    <row r="674" spans="6:6">
+      <c r="F674" s="20"/>
+    </row>
+    <row r="675" spans="6:6">
+      <c r="F675" s="20"/>
+    </row>
+    <row r="676" spans="6:6">
+      <c r="F676" s="20"/>
+    </row>
+    <row r="677" spans="6:6">
+      <c r="F677" s="20"/>
+    </row>
+    <row r="678" spans="6:6">
+      <c r="F678" s="20"/>
+    </row>
+    <row r="679" spans="6:6">
+      <c r="F679" s="20"/>
+    </row>
+    <row r="680" spans="6:6">
+      <c r="F680" s="20"/>
+    </row>
+    <row r="681" spans="6:6">
+      <c r="F681" s="20"/>
+    </row>
+    <row r="682" spans="6:6">
+      <c r="F682" s="20"/>
+    </row>
+    <row r="683" spans="6:6">
+      <c r="F683" s="20"/>
+    </row>
+    <row r="684" spans="6:6">
+      <c r="F684" s="20"/>
+    </row>
+    <row r="685" spans="6:6">
+      <c r="F685" s="20"/>
+    </row>
+    <row r="686" spans="6:6">
+      <c r="F686" s="20"/>
+    </row>
+    <row r="687" spans="6:6">
+      <c r="F687" s="20"/>
+    </row>
+    <row r="688" spans="6:6">
+      <c r="F688" s="20"/>
+    </row>
+    <row r="689" spans="6:6">
+      <c r="F689" s="20"/>
+    </row>
+    <row r="690" spans="6:6">
+      <c r="F690" s="20"/>
+    </row>
+    <row r="691" spans="6:6">
+      <c r="F691" s="20"/>
+    </row>
+    <row r="692" spans="6:6">
+      <c r="F692" s="20"/>
+    </row>
+    <row r="693" spans="6:6">
+      <c r="F693" s="20"/>
+    </row>
+    <row r="694" spans="6:6">
+      <c r="F694" s="20"/>
+    </row>
+    <row r="695" spans="6:6">
+      <c r="F695" s="20"/>
+    </row>
+    <row r="696" spans="6:6">
+      <c r="F696" s="20"/>
+    </row>
+    <row r="697" spans="6:6">
+      <c r="F697" s="20"/>
+    </row>
+    <row r="698" spans="6:6">
+      <c r="F698" s="20"/>
+    </row>
+    <row r="699" spans="6:6">
+      <c r="F699" s="20"/>
+    </row>
+    <row r="700" spans="6:6">
+      <c r="F700" s="20"/>
+    </row>
+    <row r="701" spans="6:6">
+      <c r="F701" s="20"/>
+    </row>
+    <row r="702" spans="6:6">
+      <c r="F702" s="20"/>
+    </row>
+    <row r="703" spans="6:6">
+      <c r="F703" s="20"/>
+    </row>
+    <row r="704" spans="6:6">
+      <c r="F704" s="20"/>
+    </row>
+    <row r="705" spans="6:6">
+      <c r="F705" s="20"/>
+    </row>
+    <row r="706" spans="6:6">
+      <c r="F706" s="20"/>
+    </row>
+    <row r="707" spans="6:6">
+      <c r="F707" s="20"/>
+    </row>
+    <row r="708" spans="6:6">
+      <c r="F708" s="20"/>
+    </row>
+    <row r="709" spans="6:6">
+      <c r="F709" s="20"/>
+    </row>
+    <row r="710" spans="6:6">
+      <c r="F710" s="20"/>
+    </row>
+    <row r="711" spans="6:6">
+      <c r="F711" s="20"/>
+    </row>
+    <row r="712" spans="6:6">
+      <c r="F712" s="20"/>
+    </row>
+    <row r="713" spans="6:6">
+      <c r="F713" s="20"/>
+    </row>
+    <row r="714" spans="6:6">
+      <c r="F714" s="20"/>
+    </row>
+    <row r="715" spans="6:6">
+      <c r="F715" s="20"/>
+    </row>
+    <row r="716" spans="6:6">
+      <c r="F716" s="20"/>
+    </row>
+    <row r="717" spans="6:6">
+      <c r="F717" s="20"/>
+    </row>
+    <row r="718" spans="6:6">
+      <c r="F718" s="20"/>
+    </row>
+    <row r="719" spans="6:6">
+      <c r="F719" s="20"/>
+    </row>
+    <row r="720" spans="6:6">
+      <c r="F720" s="20"/>
+    </row>
+    <row r="721" spans="6:6">
+      <c r="F721" s="20"/>
+    </row>
+    <row r="722" spans="6:6">
+      <c r="F722" s="20"/>
+    </row>
+    <row r="723" spans="6:6">
+      <c r="F723" s="20"/>
+    </row>
+    <row r="724" spans="6:6">
+      <c r="F724" s="20"/>
+    </row>
+    <row r="725" spans="6:6">
+      <c r="F725" s="20"/>
+    </row>
+    <row r="726" spans="6:6">
+      <c r="F726" s="20"/>
+    </row>
+    <row r="727" spans="6:6">
+      <c r="F727" s="20"/>
+    </row>
+    <row r="728" spans="6:6">
+      <c r="F728" s="20"/>
+    </row>
+    <row r="729" spans="6:6">
+      <c r="F729" s="20"/>
+    </row>
+    <row r="730" spans="6:6">
+      <c r="F730" s="20"/>
+    </row>
+    <row r="731" spans="6:6">
+      <c r="F731" s="20"/>
+    </row>
+    <row r="732" spans="6:6">
+      <c r="F732" s="20"/>
+    </row>
+    <row r="733" spans="6:6">
+      <c r="F733" s="20"/>
+    </row>
+    <row r="734" spans="6:6">
+      <c r="F734" s="20"/>
+    </row>
+    <row r="735" spans="6:6">
+      <c r="F735" s="20"/>
+    </row>
+    <row r="736" spans="6:6">
+      <c r="F736" s="20"/>
+    </row>
+    <row r="737" spans="6:6">
+      <c r="F737" s="20"/>
+    </row>
+    <row r="738" spans="6:6">
+      <c r="F738" s="20"/>
+    </row>
+    <row r="739" spans="6:6">
+      <c r="F739" s="20"/>
+    </row>
+    <row r="740" spans="6:6">
+      <c r="F740" s="20"/>
+    </row>
+    <row r="741" spans="6:6">
+      <c r="F741" s="20"/>
+    </row>
+    <row r="742" spans="6:6">
+      <c r="F742" s="20"/>
+    </row>
+    <row r="743" spans="6:6">
+      <c r="F743" s="20"/>
+    </row>
+    <row r="744" spans="6:6">
+      <c r="F744" s="20"/>
+    </row>
+    <row r="745" spans="6:6">
+      <c r="F745" s="20"/>
+    </row>
+    <row r="746" spans="6:6">
+      <c r="F746" s="20"/>
+    </row>
+    <row r="747" spans="6:6">
+      <c r="F747" s="20"/>
+    </row>
+    <row r="748" spans="6:6">
+      <c r="F748" s="20"/>
+    </row>
+    <row r="749" spans="6:6">
+      <c r="F749" s="20"/>
+    </row>
+    <row r="750" spans="6:6">
+      <c r="F750" s="20"/>
+    </row>
+    <row r="751" spans="6:6">
+      <c r="F751" s="20"/>
+    </row>
+    <row r="752" spans="6:6">
+      <c r="F752" s="20"/>
+    </row>
+    <row r="753" spans="6:6">
+      <c r="F753" s="20"/>
+    </row>
+    <row r="754" spans="6:6">
+      <c r="F754" s="20"/>
+    </row>
+    <row r="755" spans="6:6">
+      <c r="F755" s="20"/>
+    </row>
+    <row r="756" spans="6:6">
+      <c r="F756" s="20"/>
+    </row>
+    <row r="757" spans="6:6">
+      <c r="F757" s="20"/>
+    </row>
+    <row r="758" spans="6:6">
+      <c r="F758" s="20"/>
+    </row>
+    <row r="759" spans="6:6">
+      <c r="F759" s="20"/>
+    </row>
+    <row r="760" spans="6:6">
+      <c r="F760" s="20"/>
+    </row>
+    <row r="761" spans="6:6">
+      <c r="F761" s="20"/>
+    </row>
+    <row r="762" spans="6:6">
+      <c r="F762" s="20"/>
+    </row>
+    <row r="763" spans="6:6">
+      <c r="F763" s="20"/>
+    </row>
+    <row r="764" spans="6:6">
+      <c r="F764" s="20"/>
+    </row>
+    <row r="765" spans="6:6">
+      <c r="F765" s="20"/>
+    </row>
+    <row r="766" spans="6:6">
+      <c r="F766" s="20"/>
+    </row>
+    <row r="767" spans="6:6">
+      <c r="F767" s="20"/>
+    </row>
+    <row r="768" spans="6:6">
+      <c r="F768" s="20"/>
+    </row>
+    <row r="769" spans="6:6">
+      <c r="F769" s="20"/>
+    </row>
+    <row r="770" spans="6:6">
+      <c r="F770" s="20"/>
+    </row>
+    <row r="771" spans="6:6">
+      <c r="F771" s="20"/>
+    </row>
+    <row r="772" spans="6:6">
+      <c r="F772" s="20"/>
+    </row>
+    <row r="773" spans="6:6">
+      <c r="F773" s="20"/>
+    </row>
+    <row r="774" spans="6:6">
+      <c r="F774" s="20"/>
+    </row>
+    <row r="775" spans="6:6">
+      <c r="F775" s="20"/>
+    </row>
+    <row r="776" spans="6:6">
+      <c r="F776" s="20"/>
+    </row>
+    <row r="777" spans="6:6">
+      <c r="F777" s="20"/>
+    </row>
+    <row r="778" spans="6:6">
+      <c r="F778" s="20"/>
+    </row>
+    <row r="779" spans="6:6">
+      <c r="F779" s="20"/>
+    </row>
+    <row r="780" spans="6:6">
+      <c r="F780" s="20"/>
+    </row>
+    <row r="781" spans="6:6">
+      <c r="F781" s="19"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F23:F780"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Error messages and some validations for request reservation
</commit_message>
<xml_diff>
--- a/Project_Analysis_Team_3/Project_Analysis.xlsx
+++ b/Project_Analysis_Team_3/Project_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houda/Desktop/UTA_Parking/Project_Analysis_Team_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA528D23-54E5-A646-8D9F-497C013E2948}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B9050-4721-C947-BEDD-14B30E7836BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t>Function ID</t>
   </si>
@@ -437,12 +437,74 @@
   <si>
     <t xml:space="preserve">Parking manager sets no-show or overdue for parking user. </t>
   </si>
+  <si>
+    <t>output cannot be none</t>
+  </si>
+  <si>
+    <t>input connot be none.</t>
+  </si>
+  <si>
+    <t>input and output cannot be none</t>
+  </si>
+  <si>
+    <t>input and output connot be none.</t>
+  </si>
+  <si>
+    <t>Output invalid</t>
+  </si>
+  <si>
+    <t>Input invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3c- 3d- 3e </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA COMMENTS </t>
+  </si>
+  <si>
+    <t>Comments to TA</t>
+  </si>
+  <si>
+    <t>THE OUTPUT IS EXACTLY THE ONE THE PROFESSOR USED IN EXAMPLE FUNCTION LIST.</t>
+  </si>
+  <si>
+    <t>THE INPUT/OUTPUT IS EXACTLY THE ONE THE PROFESSOR USED IN EXAMPLE FUNCTION LIST.
+He also said in class that we shall not list buttons as inputs which is the case here. The user selects a button which displays (outputs) the infornation to be modified. The outputs are modifiable put the input to access the function was just a click.</t>
+  </si>
+  <si>
+    <t>The user does not provide any data. That was the definition of input that professor said. If the user enters something manually it is input if not list it as none.</t>
+  </si>
+  <si>
+    <t>The user does not provide any data. That was the definition of input that professor said. If the user enters something manually it is input if not list it as none. NO DATA IS PROVIDED NO DATA IS DISPLAYED. I SPECIFICALLY ASKED THE PROFESSOR IF SELECTING AN ITEM FROM A LIST IS CONSIDERED INPUT HE SAID NO. Inputs are what the user ENTERS</t>
+  </si>
+  <si>
+    <t>THE INPUT/OUTPUT IS EXACTLY THE ONE THE PROFESSOR USED IN EXAMPLE FUNCTION LIST for update profile.
+He also said in class that we shall not list buttons as inputs which is the case here. The user selects a button which displays (outputs) the infornation to be modified. The outputs are modifiable put the input to access the function was just a click.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHY? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO DATA IS DISPLAYED TO USER AS PER PROFESSOR S DEFINITION OF OUTPUT&gt; </t>
+  </si>
+  <si>
+    <t>NO DATA IS DISPLAYED TO USER AS PER PROFESSOR S DEFINITION OF OUTPUT. Screens are not outputs.</t>
+  </si>
+  <si>
+    <t>SEARCH BY USERNAME IS OUTPUT. Outputs are not data, there are BUTTONS. We were asked not to specify clicking on buttons.</t>
+  </si>
+  <si>
+    <t>SAME AS UPDATE PROFILE. JUST LIKE PROFESSOR S EXAMPLE.</t>
+  </si>
+  <si>
+    <t>THOSE ARE COMBINED. PROFESSOR SAID THAT THOSE ARE FUNCTIONNALITIES NOT FUNCTIONS SEPARATELY. MODIFY ROLE AND SET STATUS ACTIVE OR REVOKED AND REASON FOR VIOLATION ARE IMPLIED IN THE ATTRIBUTE LISTED IN OUTPUTS THAN CAN BE CHANGED.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,8 +539,22 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +570,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -610,6 +698,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,20 +1048,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24"/>
   <cols>
     <col min="1" max="1" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="48" style="18" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="59" width="8.83203125" style="12"/>
+    <col min="8" max="8" width="25.1640625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="12"/>
+    <col min="10" max="10" width="35.5" style="23" customWidth="1"/>
+    <col min="11" max="59" width="8.83203125" style="12"/>
     <col min="60" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -987,9 +1087,13 @@
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="J1" s="22" t="s">
+        <v>85</v>
+      </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
@@ -1059,8 +1163,14 @@
       <c r="F2" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:59" ht="60">
+      <c r="H2" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" ht="100">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1079,8 +1189,14 @@
       <c r="F3" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:59" ht="60">
+      <c r="H3" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" ht="100">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1099,8 +1215,14 @@
       <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:59" ht="80">
+      <c r="H4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" ht="375">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1119,8 +1241,14 @@
       <c r="F5" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:59" ht="160">
+      <c r="H5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="140">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1140,7 +1268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="160">
+    <row r="7" spans="1:59" ht="175">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1159,8 +1287,14 @@
       <c r="F7" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:59" ht="80">
+      <c r="H7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" ht="175">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1179,8 +1313,14 @@
       <c r="F8" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:59" ht="40">
+      <c r="H8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" ht="375">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1199,8 +1339,14 @@
       <c r="F9" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:59" ht="80">
+      <c r="H9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" ht="400">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1218,6 +1364,12 @@
       </c>
       <c r="F10" s="11" t="s">
         <v>57</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:59" ht="40">
@@ -1240,6 +1392,12 @@
         <v>44</v>
       </c>
       <c r="G11" s="2"/>
+      <c r="H11" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:59" ht="100">
       <c r="A12" s="8">
@@ -1300,8 +1458,14 @@
       <c r="F14" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:59" ht="120">
+      <c r="H14" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" ht="125">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1319,6 +1483,12 @@
       </c>
       <c r="F15" s="9" t="s">
         <v>36</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:59" ht="100">
@@ -1341,7 +1511,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="180">
+    <row r="17" spans="1:10" ht="180">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1362,7 +1532,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="40">
+    <row r="18" spans="1:10" ht="150">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1382,8 +1552,14 @@
         <v>76</v>
       </c>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="140">
+      <c r="H18" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="140">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1403,8 +1579,14 @@
         <v>40</v>
       </c>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="40">
+      <c r="H19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="375">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1423,8 +1605,14 @@
       <c r="F20" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="120">
+      <c r="H20" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="120">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1444,8 +1632,14 @@
         <v>61</v>
       </c>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="160">
+      <c r="H21" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="325">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1464,67 +1658,73 @@
       <c r="F22" s="9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1">
+      <c r="H22" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1">
+    <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1">
+    <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="20"/>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1">
+    <row r="26" spans="1:10" ht="15" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1">
+    <row r="27" spans="1:10" ht="15" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1">
+    <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1">
+    <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1">
+    <row r="30" spans="1:10" ht="15" customHeight="1">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1">
+    <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1">
+    <row r="32" spans="1:10" ht="15" customHeight="1">
       <c r="F32" s="20"/>
     </row>
     <row r="33" spans="6:6" ht="15" customHeight="1">

</xml_diff>